<commit_message>
update instructions and results
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/cornstover/_Li_et_al_2020/_feedstock_composition_for_simulation.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/cornstover/_Li_et_al_2020/_feedstock_composition_for_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/OneDrive/Coding/biosteam modules/lignin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/cornstover/_Li_et_al_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:40009_{C47F1679-B252-2A43-8AEA-97B9D36A83E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BE08DE44-06E5-AF4C-AABC-914E9BF710C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFBC67F-FC87-644E-9162-CE7BDC2E232E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8760" yWindow="1200" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -480,6 +480,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -525,8 +540,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -885,22 +901,22 @@
   <dimension ref="A1:D282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>